<commit_message>
Prawie dobrze, kilka mniejszych błędów
</commit_message>
<xml_diff>
--- a/Text_Files/słówka_ang_dane.xlsx
+++ b/Text_Files/słówka_ang_dane.xlsx
@@ -476,16 +476,16 @@
   </sheetPr>
   <dimension ref="A1:H2752"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A553" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F568" activeCellId="0" sqref="F568"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A754" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E772" activeCellId="0" sqref="E772"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.61328125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.625" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="24.47" customWidth="1" style="4" min="2" max="2"/>
     <col width="19.48" customWidth="1" style="4" min="3" max="3"/>
     <col width="22.73" customWidth="1" style="4" min="4" max="4"/>
-    <col width="32.59" customWidth="1" style="4" min="5" max="5"/>
+    <col width="32.6" customWidth="1" style="4" min="5" max="5"/>
     <col width="39.09" customWidth="1" style="4" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -893,10 +893,10 @@
         </is>
       </c>
       <c r="G12" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H12" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" ht="15" customHeight="1" s="5">
@@ -939,10 +939,10 @@
         </is>
       </c>
       <c r="G14" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H14" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" ht="15" customHeight="1" s="5">
@@ -967,10 +967,10 @@
         </is>
       </c>
       <c r="G15" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H15" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" ht="15" customHeight="1" s="5">
@@ -995,10 +995,10 @@
         </is>
       </c>
       <c r="G16" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" ht="15" customHeight="1" s="5">
@@ -1023,10 +1023,10 @@
         </is>
       </c>
       <c r="G17" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H17" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" ht="15" customHeight="1" s="5">
@@ -1051,10 +1051,10 @@
         </is>
       </c>
       <c r="G18" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H18" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" ht="15" customHeight="1" s="5">
@@ -1065,7 +1065,7 @@
       </c>
       <c r="B19" s="4" t="inlineStr">
         <is>
-          <t>albo</t>
+          <t>albo, którykolwiek</t>
         </is>
       </c>
       <c r="C19" s="4" t="inlineStr">
@@ -1079,10 +1079,10 @@
         </is>
       </c>
       <c r="G19" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" ht="15" customHeight="1" s="5">
@@ -1107,10 +1107,10 @@
         </is>
       </c>
       <c r="G20" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" ht="15" customHeight="1" s="5">
@@ -1135,10 +1135,10 @@
         </is>
       </c>
       <c r="G21" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H21" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" ht="15" customHeight="1" s="5">
@@ -1163,10 +1163,10 @@
         </is>
       </c>
       <c r="G22" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H22" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" ht="15" customHeight="1" s="5">
@@ -1191,10 +1191,10 @@
         </is>
       </c>
       <c r="G23" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" ht="15" customHeight="1" s="5">
@@ -1219,10 +1219,10 @@
         </is>
       </c>
       <c r="G24" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H24" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" ht="15" customHeight="1" s="5">
@@ -1233,7 +1233,7 @@
       </c>
       <c r="B25" s="4" t="inlineStr">
         <is>
-          <t>ani</t>
+          <t>ani ( w kontekście łączone z either)</t>
         </is>
       </c>
       <c r="C25" s="4" t="inlineStr">
@@ -1247,10 +1247,10 @@
         </is>
       </c>
       <c r="G25" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" ht="15" customHeight="1" s="5">
@@ -1275,10 +1275,10 @@
         </is>
       </c>
       <c r="G26" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" ht="15" customHeight="1" s="5">
@@ -1303,10 +1303,10 @@
         </is>
       </c>
       <c r="G27" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H27" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" ht="15" customHeight="1" s="5">
@@ -1331,10 +1331,10 @@
         </is>
       </c>
       <c r="G28" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" ht="15" customHeight="1" s="5">
@@ -1359,10 +1359,10 @@
         </is>
       </c>
       <c r="G29" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" ht="15" customHeight="1" s="5">
@@ -1387,10 +1387,10 @@
         </is>
       </c>
       <c r="G30" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" ht="15" customHeight="1" s="5">
@@ -1415,10 +1415,10 @@
         </is>
       </c>
       <c r="G31" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H31" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" ht="15" customHeight="1" s="5">
@@ -1443,10 +1443,10 @@
         </is>
       </c>
       <c r="G32" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H32" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" ht="15" customHeight="1" s="5">
@@ -1471,10 +1471,10 @@
         </is>
       </c>
       <c r="G33" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H33" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" ht="15" customHeight="1" s="5">
@@ -1499,10 +1499,10 @@
         </is>
       </c>
       <c r="G34" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H34" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" ht="15" customHeight="1" s="5">
@@ -1527,10 +1527,10 @@
         </is>
       </c>
       <c r="G35" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" ht="15" customHeight="1" s="5">
@@ -1555,10 +1555,10 @@
         </is>
       </c>
       <c r="G36" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H36" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" ht="15" customHeight="1" s="5">
@@ -1583,10 +1583,10 @@
         </is>
       </c>
       <c r="G37" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H37" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" ht="15" customHeight="1" s="5">
@@ -1649,10 +1649,10 @@
         </is>
       </c>
       <c r="G39" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H39" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" ht="15" customHeight="1" s="5">
@@ -1677,10 +1677,10 @@
         </is>
       </c>
       <c r="G40" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H40" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" ht="15" customHeight="1" s="5">
@@ -1705,10 +1705,10 @@
         </is>
       </c>
       <c r="G41" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H41" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" ht="15" customHeight="1" s="5">
@@ -1733,10 +1733,10 @@
         </is>
       </c>
       <c r="G42" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H42" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" ht="15" customHeight="1" s="5">
@@ -1761,10 +1761,10 @@
         </is>
       </c>
       <c r="G43" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H43" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" ht="15" customHeight="1" s="5">
@@ -1789,10 +1789,10 @@
         </is>
       </c>
       <c r="G44" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H44" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" ht="15" customHeight="1" s="5">
@@ -1811,16 +1811,26 @@
           <t>Asian</t>
         </is>
       </c>
+      <c r="D45" s="4" t="inlineStr">
+        <is>
+          <t>Azjata z Azji</t>
+        </is>
+      </c>
+      <c r="E45" s="4" t="inlineStr">
+        <is>
+          <t>Asian from Asia</t>
+        </is>
+      </c>
       <c r="F45" s="4" t="inlineStr">
         <is>
           <t>C:\Users\admin\Documents\ANGIELSKI\Angielski do słuchania\Asian.mp3</t>
         </is>
       </c>
       <c r="G45" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H45" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" ht="15" customHeight="1" s="5">
@@ -1845,10 +1855,10 @@
         </is>
       </c>
       <c r="G46" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H46" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" ht="15" customHeight="1" s="5">
@@ -1867,16 +1877,26 @@
           <t>researcher</t>
         </is>
       </c>
+      <c r="D47" s="4" t="inlineStr">
+        <is>
+          <t>badacz naukowy</t>
+        </is>
+      </c>
+      <c r="E47" s="4" t="inlineStr">
+        <is>
+          <t>scientific researcher</t>
+        </is>
+      </c>
       <c r="F47" s="4" t="inlineStr">
         <is>
           <t>C:\Users\admin\Documents\ANGIELSKI\Angielski do słuchania\researcher.mp3</t>
         </is>
       </c>
       <c r="G47" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H47" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" ht="15" customHeight="1" s="5">
@@ -1887,7 +1907,7 @@
       </c>
       <c r="B48" s="4" t="inlineStr">
         <is>
-          <t>badać</t>
+          <t>badać(inaczej odkrywać lub zwiedzać)</t>
         </is>
       </c>
       <c r="C48" s="4" t="inlineStr">
@@ -1901,10 +1921,10 @@
         </is>
       </c>
       <c r="G48" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H48" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" ht="15" customHeight="1" s="5">
@@ -1929,10 +1949,10 @@
         </is>
       </c>
       <c r="G49" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H49" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" ht="15" customHeight="1" s="5">
@@ -1943,7 +1963,7 @@
       </c>
       <c r="B50" s="4" t="inlineStr">
         <is>
-          <t>badanie</t>
+          <t>badanie(jako opracowanie, analiza)</t>
         </is>
       </c>
       <c r="C50" s="4" t="inlineStr">
@@ -1957,10 +1977,10 @@
         </is>
       </c>
       <c r="G50" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H50" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" ht="15" customHeight="1" s="5">
@@ -1985,10 +2005,10 @@
         </is>
       </c>
       <c r="G51" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H51" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" ht="15" customHeight="1" s="5">
@@ -2013,10 +2033,10 @@
         </is>
       </c>
       <c r="G52" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H52" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" ht="15" customHeight="1" s="5">
@@ -2041,10 +2061,10 @@
         </is>
       </c>
       <c r="G53" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H53" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" ht="15" customHeight="1" s="5">
@@ -2069,10 +2089,10 @@
         </is>
       </c>
       <c r="G54" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H54" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" ht="15" customHeight="1" s="5">
@@ -2091,16 +2111,26 @@
           <t>barrel</t>
         </is>
       </c>
+      <c r="D55" s="4" t="inlineStr">
+        <is>
+          <t>pełny baryłka oleju</t>
+        </is>
+      </c>
+      <c r="E55" s="4" t="inlineStr">
+        <is>
+          <t>full barrel of oil</t>
+        </is>
+      </c>
       <c r="F55" s="4" t="inlineStr">
         <is>
           <t>C:\Users\admin\Documents\ANGIELSKI\Angielski do słuchania\barrel.mp3</t>
         </is>
       </c>
       <c r="G55" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H55" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" ht="15" customHeight="1" s="5">
@@ -2125,10 +2155,10 @@
         </is>
       </c>
       <c r="G56" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H56" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" ht="15" customHeight="1" s="5">
@@ -2153,10 +2183,10 @@
         </is>
       </c>
       <c r="G57" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H57" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" ht="15" customHeight="1" s="5">
@@ -2181,10 +2211,10 @@
         </is>
       </c>
       <c r="G58" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H58" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" ht="15" customHeight="1" s="5">
@@ -2209,10 +2239,10 @@
         </is>
       </c>
       <c r="G59" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H59" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" ht="15" customHeight="1" s="5">
@@ -2237,10 +2267,10 @@
         </is>
       </c>
       <c r="G60" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H60" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" ht="15" customHeight="1" s="5">
@@ -2265,10 +2295,10 @@
         </is>
       </c>
       <c r="G61" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H61" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" ht="15" customHeight="1" s="5">
@@ -2293,10 +2323,10 @@
         </is>
       </c>
       <c r="G62" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H62" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" ht="15" customHeight="1" s="5">
@@ -2321,10 +2351,10 @@
         </is>
       </c>
       <c r="G63" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H63" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" ht="15" customHeight="1" s="5">
@@ -2349,10 +2379,10 @@
         </is>
       </c>
       <c r="G64" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H64" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" ht="15" customHeight="1" s="5">
@@ -2395,10 +2425,10 @@
         </is>
       </c>
       <c r="G66" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H66" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" ht="15" customHeight="1" s="5">
@@ -2417,16 +2447,26 @@
           <t>direct</t>
         </is>
       </c>
+      <c r="D67" s="4" t="inlineStr">
+        <is>
+          <t>bezpośrednia rozmowa</t>
+        </is>
+      </c>
+      <c r="E67" s="4" t="inlineStr">
+        <is>
+          <t>direct conversation</t>
+        </is>
+      </c>
       <c r="F67" s="4" t="inlineStr">
         <is>
           <t>C:\Users\admin\Documents\ANGIELSKI\Angielski do słuchania\direct.mp3</t>
         </is>
       </c>
       <c r="G67" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H67" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" ht="15" customHeight="1" s="5">
@@ -2445,16 +2485,26 @@
           <t>directly</t>
         </is>
       </c>
+      <c r="D68" s="4" t="inlineStr">
+        <is>
+          <t>Idź bezpośrednio do domu</t>
+        </is>
+      </c>
+      <c r="E68" s="4" t="inlineStr">
+        <is>
+          <t>Go directly home</t>
+        </is>
+      </c>
       <c r="F68" s="4" t="inlineStr">
         <is>
           <t>C:\Users\admin\Documents\ANGIELSKI\Angielski do słuchania\directly.mp3</t>
         </is>
       </c>
       <c r="G68" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H68" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" ht="15" customHeight="1" s="5">
@@ -2479,10 +2529,10 @@
         </is>
       </c>
       <c r="G69" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H69" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" ht="15" customHeight="1" s="5">
@@ -2507,10 +2557,10 @@
         </is>
       </c>
       <c r="G70" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H70" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" ht="15" customHeight="1" s="5">
@@ -2535,10 +2585,10 @@
         </is>
       </c>
       <c r="G71" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H71" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" ht="15" customHeight="1" s="5">
@@ -2563,10 +2613,10 @@
         </is>
       </c>
       <c r="G72" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H72" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" ht="15" customHeight="1" s="5">
@@ -2592,7 +2642,7 @@
       </c>
       <c r="E73" s="4" t="inlineStr">
         <is>
-          <t>They beat him until he was unconscious.</t>
+          <t>They beat him unconscious.</t>
         </is>
       </c>
       <c r="F73" s="4" t="inlineStr">
@@ -2601,10 +2651,10 @@
         </is>
       </c>
       <c r="G73" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H73" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" ht="15" customHeight="1" s="5">
@@ -2629,10 +2679,10 @@
         </is>
       </c>
       <c r="G74" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H74" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" ht="15" customHeight="1" s="5">
@@ -2643,7 +2693,7 @@
       </c>
       <c r="B75" s="4" t="inlineStr">
         <is>
-          <t>bieżący</t>
+          <t>trwający</t>
         </is>
       </c>
       <c r="C75" s="4" t="inlineStr">
@@ -2667,10 +2717,10 @@
         </is>
       </c>
       <c r="G75" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H75" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" ht="15" customHeight="1" s="5">
@@ -19886,7 +19936,6 @@
           <t>I have no other ideas</t>
         </is>
       </c>
-      <c r="F568" s="4" t="n"/>
       <c r="G568" s="4" t="n">
         <v>1</v>
       </c>
@@ -23654,13 +23703,18 @@
         </is>
       </c>
       <c r="G680" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H680" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="681" ht="15" customHeight="1" s="5">
+      <c r="A681" s="4" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
       <c r="B681" s="4" t="inlineStr">
         <is>
           <t>kłopoty</t>
@@ -23673,19 +23727,24 @@
       </c>
       <c r="D681" s="4" t="inlineStr">
         <is>
-          <t>kłopoty w pracy</t>
+          <t>kwadratowa plansza</t>
         </is>
       </c>
       <c r="E681" s="4" t="inlineStr">
         <is>
-          <t>trouble at work</t>
+          <t>square board</t>
+        </is>
+      </c>
+      <c r="F681" s="4" t="inlineStr">
+        <is>
+          <t>C:\Users\admin\Documents\ANGIELSKI\Angielski do słuchania\trouble.mp3</t>
         </is>
       </c>
       <c r="G681" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H681" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="682" ht="15" customHeight="1" s="5">
@@ -24218,10 +24277,10 @@
         </is>
       </c>
       <c r="G698" s="4" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H698" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="699" ht="15" customHeight="1" s="5">
@@ -25598,10 +25657,10 @@
         </is>
       </c>
       <c r="G738" s="4" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H738" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="739" ht="15" customHeight="1" s="5">
@@ -25626,10 +25685,10 @@
         </is>
       </c>
       <c r="G739" s="4" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H739" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="740" ht="15" customHeight="1" s="5">
@@ -25956,10 +26015,10 @@
         </is>
       </c>
       <c r="G749" s="4" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H749" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="750" ht="15" customHeight="1" s="5">
@@ -25984,10 +26043,10 @@
         </is>
       </c>
       <c r="G750" s="4" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H750" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="751" ht="15" customHeight="1" s="5">
@@ -26050,10 +26109,10 @@
         </is>
       </c>
       <c r="G752" s="4" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H752" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="753" ht="15" customHeight="1" s="5">
@@ -26095,6 +26154,11 @@
       </c>
     </row>
     <row r="754" ht="15" customHeight="1" s="5">
+      <c r="A754" s="4" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
       <c r="B754" s="4" t="inlineStr">
         <is>
           <t>koszt</t>
@@ -26112,14 +26176,19 @@
       </c>
       <c r="E754" s="4" t="inlineStr">
         <is>
-          <t>reduce expenses</t>
+          <t>reduce costs</t>
+        </is>
+      </c>
+      <c r="F754" s="4" t="inlineStr">
+        <is>
+          <t>C:\Users\admin\Documents\ANGIELSKI\Angielski do słuchania\expense.mp3</t>
         </is>
       </c>
       <c r="G754" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H754" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="755" ht="15" customHeight="1" s="5">
@@ -26144,10 +26213,10 @@
         </is>
       </c>
       <c r="G755" s="4" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H755" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="756" ht="15" customHeight="1" s="5">
@@ -26172,10 +26241,10 @@
         </is>
       </c>
       <c r="G756" s="4" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H756" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="757" ht="15" customHeight="1" s="5">
@@ -26228,10 +26297,10 @@
         </is>
       </c>
       <c r="G758" s="4" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H758" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="759" ht="15" customHeight="1" s="5">
@@ -26256,10 +26325,10 @@
         </is>
       </c>
       <c r="G759" s="4" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H759" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="760" ht="15" customHeight="1" s="5">
@@ -26312,10 +26381,10 @@
         </is>
       </c>
       <c r="G761" s="4" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H761" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="762" ht="15" customHeight="1" s="5">
@@ -26368,10 +26437,10 @@
         </is>
       </c>
       <c r="G763" s="4" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H763" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="764" ht="15" customHeight="1" s="5">
@@ -26462,10 +26531,10 @@
         </is>
       </c>
       <c r="G766" s="4" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H766" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="767" ht="15" customHeight="1" s="5">
@@ -26497,6 +26566,11 @@
       </c>
     </row>
     <row r="768" ht="15" customHeight="1" s="5">
+      <c r="A768" s="4" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
       <c r="B768" s="4" t="inlineStr">
         <is>
           <t>kreacja</t>
@@ -26509,19 +26583,24 @@
       </c>
       <c r="D768" s="4" t="inlineStr">
         <is>
-          <t>dzieło sztuki, kreacja</t>
+          <t>dzielo</t>
         </is>
       </c>
       <c r="E768" s="4" t="inlineStr">
         <is>
-          <t>work of art, creation</t>
+          <t>creation</t>
+        </is>
+      </c>
+      <c r="F768" s="4" t="inlineStr">
+        <is>
+          <t>C:\Users\admin\Documents\ANGIELSKI\Angielski do słuchania\creation.mp3</t>
         </is>
       </c>
       <c r="G768" s="4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H768" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="769" ht="15" customHeight="1" s="5">
@@ -27232,10 +27311,10 @@
         </is>
       </c>
       <c r="G791" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H791" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="792" ht="15" customHeight="1" s="5">
@@ -27260,10 +27339,10 @@
         </is>
       </c>
       <c r="G792" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H792" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="793" ht="15" customHeight="1" s="5">
@@ -27288,10 +27367,10 @@
         </is>
       </c>
       <c r="G793" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H793" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="794" ht="15" customHeight="1" s="5">
@@ -27316,10 +27395,10 @@
         </is>
       </c>
       <c r="G794" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H794" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="795" ht="15" customHeight="1" s="5">
@@ -27344,10 +27423,10 @@
         </is>
       </c>
       <c r="G795" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H795" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="796" ht="15" customHeight="1" s="5">
@@ -27603,6 +27682,11 @@
       </c>
     </row>
     <row r="805" ht="15" customHeight="1" s="5">
+      <c r="A805" s="4" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
       <c r="B805" s="4" t="inlineStr">
         <is>
           <t>kupujący</t>
@@ -27615,19 +27699,24 @@
       </c>
       <c r="D805" s="4" t="inlineStr">
         <is>
-          <t>potencjalny kupujący</t>
+          <t>nowy kupujący</t>
         </is>
       </c>
       <c r="E805" s="4" t="inlineStr">
         <is>
-          <t>potential buyer</t>
+          <t>new buyer</t>
+        </is>
+      </c>
+      <c r="F805" s="4" t="inlineStr">
+        <is>
+          <t>C:\Users\admin\Documents\ANGIELSKI\Angielski do słuchania\buyer.mp3</t>
         </is>
       </c>
       <c r="G805" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H805" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="806" ht="15" customHeight="1" s="5">
@@ -27652,10 +27741,10 @@
         </is>
       </c>
       <c r="G806" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H806" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="807" ht="15" customHeight="1" s="5">
@@ -27680,10 +27769,10 @@
         </is>
       </c>
       <c r="G807" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H807" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="808" ht="15" customHeight="1" s="5">
@@ -27708,13 +27797,18 @@
         </is>
       </c>
       <c r="G808" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H808" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="809" ht="15" customHeight="1" s="5">
+      <c r="A809" s="4" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
       <c r="B809" s="4" t="inlineStr">
         <is>
           <t>kuzyn</t>
@@ -27727,7 +27821,7 @@
       </c>
       <c r="D809" s="4" t="inlineStr">
         <is>
-          <t>starszy kuzyn</t>
+          <t>badacz naukowy</t>
         </is>
       </c>
       <c r="E809" s="4" t="inlineStr">
@@ -27735,14 +27829,24 @@
           <t>older cousin</t>
         </is>
       </c>
+      <c r="F809" s="4" t="inlineStr">
+        <is>
+          <t>C:\Users\admin\Documents\ANGIELSKI\Angielski do słuchania\cousin.mp3</t>
+        </is>
+      </c>
       <c r="G809" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H809" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="810" ht="15" customHeight="1" s="5">
+      <c r="A810" s="4" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
       <c r="B810" s="4" t="inlineStr">
         <is>
           <t>kwadrat</t>
@@ -27755,22 +27859,32 @@
       </c>
       <c r="D810" s="4" t="inlineStr">
         <is>
-          <t>kwadratowy stół</t>
+          <t>kwadratowa plansza</t>
         </is>
       </c>
       <c r="E810" s="4" t="inlineStr">
         <is>
-          <t>square table</t>
+          <t>square board</t>
+        </is>
+      </c>
+      <c r="F810" s="4" t="inlineStr">
+        <is>
+          <t>C:\Users\admin\Documents\ANGIELSKI\Angielski do słuchania\square.mp3</t>
         </is>
       </c>
       <c r="G810" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H810" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="811" ht="15" customHeight="1" s="5">
+      <c r="A811" s="4" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
       <c r="B811" s="4" t="inlineStr">
         <is>
           <t>kwartał</t>
@@ -27783,7 +27897,7 @@
       </c>
       <c r="D811" s="4" t="inlineStr">
         <is>
-          <t>końcówka kwartału</t>
+          <t>nowy kupujący</t>
         </is>
       </c>
       <c r="E811" s="4" t="inlineStr">
@@ -27791,11 +27905,16 @@
           <t>quarter end</t>
         </is>
       </c>
+      <c r="F811" s="4" t="inlineStr">
+        <is>
+          <t>C:\Users\admin\Documents\ANGIELSKI\Angielski do słuchania\quarter.mp3</t>
+        </is>
+      </c>
       <c r="G811" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H811" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="812" ht="15" customHeight="1" s="5">
@@ -27820,10 +27939,10 @@
         </is>
       </c>
       <c r="G812" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H812" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="813" ht="15" customHeight="1" s="5">
@@ -27848,10 +27967,10 @@
         </is>
       </c>
       <c r="G813" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H813" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="814" ht="15" customHeight="1" s="5">
@@ -27876,13 +27995,18 @@
         </is>
       </c>
       <c r="G814" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H814" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="815" ht="15" customHeight="1" s="5">
+      <c r="A815" s="4" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
       <c r="B815" s="4" t="inlineStr">
         <is>
           <t>lada</t>
@@ -27895,19 +28019,24 @@
       </c>
       <c r="D815" s="4" t="inlineStr">
         <is>
-          <t>lada sklepowa</t>
+          <t>przekąski są na ladzie</t>
         </is>
       </c>
       <c r="E815" s="4" t="inlineStr">
         <is>
-          <t>store counter</t>
+          <t>The snacks are on the counter</t>
+        </is>
+      </c>
+      <c r="F815" s="4" t="inlineStr">
+        <is>
+          <t>C:\Users\admin\Documents\ANGIELSKI\Angielski do słuchania\counter.mp3</t>
         </is>
       </c>
       <c r="G815" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H815" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="816" ht="15" customHeight="1" s="5">
@@ -27932,10 +28061,10 @@
         </is>
       </c>
       <c r="G816" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H816" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="817" ht="15" customHeight="1" s="5">
@@ -27960,10 +28089,10 @@
         </is>
       </c>
       <c r="G817" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H817" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="818" ht="15" customHeight="1" s="5">
@@ -27988,13 +28117,18 @@
         </is>
       </c>
       <c r="G818" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H818" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="819" ht="15" customHeight="1" s="5">
+      <c r="A819" s="4" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
       <c r="B819" s="4" t="inlineStr">
         <is>
           <t>lecz</t>
@@ -28007,7 +28141,7 @@
       </c>
       <c r="D819" s="4" t="inlineStr">
         <is>
-          <t>lecz nie zawsze</t>
+          <t>kwadratowa plansza</t>
         </is>
       </c>
       <c r="E819" s="4" t="inlineStr">
@@ -28015,11 +28149,16 @@
           <t>but not always</t>
         </is>
       </c>
+      <c r="F819" s="4" t="inlineStr">
+        <is>
+          <t>C:\Users\admin\Documents\ANGIELSKI\Angielski do słuchania\but.mp3</t>
+        </is>
+      </c>
       <c r="G819" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H819" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="820" ht="15" customHeight="1" s="5">
@@ -28044,16 +28183,21 @@
         </is>
       </c>
       <c r="G820" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H820" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="821" ht="15" customHeight="1" s="5">
+      <c r="A821" s="4" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
       <c r="B821" s="4" t="inlineStr">
         <is>
-          <t>ledwie</t>
+          <t>ledwie(praktycznie nie)</t>
         </is>
       </c>
       <c r="C821" s="4" t="inlineStr">
@@ -28063,22 +28207,32 @@
       </c>
       <c r="D821" s="4" t="inlineStr">
         <is>
-          <t>ledwie żywy</t>
+          <t>Ledwo przeżył</t>
         </is>
       </c>
       <c r="E821" s="4" t="inlineStr">
         <is>
-          <t>hardly alive</t>
+          <t>He hardly survived</t>
+        </is>
+      </c>
+      <c r="F821" s="4" t="inlineStr">
+        <is>
+          <t>C:\Users\admin\Documents\ANGIELSKI\Angielski do słuchania\hardly.mp3</t>
         </is>
       </c>
       <c r="G821" s="4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H821" s="4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="822" ht="15" customHeight="1" s="5">
+      <c r="A822" s="4" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
       <c r="B822" s="4" t="inlineStr">
         <is>
           <t>ledwo</t>
@@ -28091,7 +28245,7 @@
       </c>
       <c r="D822" s="4" t="inlineStr">
         <is>
-          <t>ledwo zdążyłem</t>
+          <t>kwadratowa plansza</t>
         </is>
       </c>
       <c r="E822" s="4" t="inlineStr">
@@ -28099,11 +28253,16 @@
           <t>barely made it</t>
         </is>
       </c>
+      <c r="F822" s="4" t="inlineStr">
+        <is>
+          <t>C:\Users\admin\Documents\ANGIELSKI\Angielski do słuchania\barely.mp3</t>
+        </is>
+      </c>
       <c r="G822" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H822" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="823" ht="15" customHeight="1" s="5">
@@ -28128,13 +28287,18 @@
         </is>
       </c>
       <c r="G823" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H823" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="824" ht="15" customHeight="1" s="5">
+      <c r="A824" s="4" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
       <c r="B824" s="4" t="inlineStr">
         <is>
           <t>lek</t>
@@ -28147,7 +28311,7 @@
       </c>
       <c r="D824" s="4" t="inlineStr">
         <is>
-          <t>silny lek</t>
+          <t>kwadratowa plansza</t>
         </is>
       </c>
       <c r="E824" s="4" t="inlineStr">
@@ -28155,11 +28319,16 @@
           <t>strong medication</t>
         </is>
       </c>
+      <c r="F824" s="4" t="inlineStr">
+        <is>
+          <t>C:\Users\admin\Documents\ANGIELSKI\Angielski do słuchania\medication.mp3</t>
+        </is>
+      </c>
       <c r="G824" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H824" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="825" ht="15" customHeight="1" s="5">
@@ -28184,16 +28353,16 @@
         </is>
       </c>
       <c r="G825" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H825" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="826" ht="15" customHeight="1" s="5">
       <c r="B826" s="4" t="inlineStr">
         <is>
-          <t>Lekarz</t>
+          <t>Lekarz(medycyny)</t>
         </is>
       </c>
       <c r="C826" s="4" t="inlineStr">
@@ -28212,10 +28381,10 @@
         </is>
       </c>
       <c r="G826" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H826" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="827" ht="15" customHeight="1" s="5">
@@ -28240,10 +28409,10 @@
         </is>
       </c>
       <c r="G827" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H827" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="828" ht="15" customHeight="1" s="5">
@@ -28268,10 +28437,10 @@
         </is>
       </c>
       <c r="G828" s="4" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H828" s="4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="829" ht="15" customHeight="1" s="5">
@@ -28296,10 +28465,10 @@
         </is>
       </c>
       <c r="G829" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H829" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="830" ht="15" customHeight="1" s="5">
@@ -28324,10 +28493,10 @@
         </is>
       </c>
       <c r="G830" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H830" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="831" ht="15" customHeight="1" s="5">
@@ -28380,10 +28549,10 @@
         </is>
       </c>
       <c r="G832" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H832" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="833" ht="15" customHeight="1" s="5">
@@ -28408,10 +28577,10 @@
         </is>
       </c>
       <c r="G833" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H833" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="834" ht="15" customHeight="1" s="5">
@@ -28436,10 +28605,10 @@
         </is>
       </c>
       <c r="G834" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H834" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="835" ht="15" customHeight="1" s="5">
@@ -28464,10 +28633,10 @@
         </is>
       </c>
       <c r="G835" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H835" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="836" ht="15" customHeight="1" s="5">
@@ -28530,10 +28699,10 @@
         </is>
       </c>
       <c r="G837" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H837" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="838" ht="15" customHeight="1" s="5">
@@ -28558,10 +28727,10 @@
         </is>
       </c>
       <c r="G838" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H838" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="839" ht="15" customHeight="1" s="5">
@@ -28586,10 +28755,10 @@
         </is>
       </c>
       <c r="G839" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H839" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="840" ht="15" customHeight="1" s="5">
@@ -28652,10 +28821,10 @@
         </is>
       </c>
       <c r="G841" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H841" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="842" ht="15" customHeight="1" s="5">
@@ -28680,10 +28849,10 @@
         </is>
       </c>
       <c r="G842" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H842" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="843" ht="15" customHeight="1" s="5">
@@ -28784,10 +28953,10 @@
         </is>
       </c>
       <c r="G845" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H845" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="846" ht="15" customHeight="1" s="5">
@@ -28812,10 +28981,10 @@
         </is>
       </c>
       <c r="G846" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H846" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="847" ht="15" customHeight="1" s="5">
@@ -28840,13 +29009,18 @@
         </is>
       </c>
       <c r="G847" s="4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H847" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="848" ht="15" customHeight="1" s="5">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
       <c r="B848" s="4" t="inlineStr">
         <is>
           <t>los</t>
@@ -28859,19 +29033,24 @@
       </c>
       <c r="D848" s="4" t="inlineStr">
         <is>
-          <t>zmienić los</t>
+          <t>zadecydowały okoliczności losu</t>
         </is>
       </c>
       <c r="E848" s="4" t="inlineStr">
         <is>
-          <t>change fate</t>
+          <t>The circumstances of fate decided</t>
+        </is>
+      </c>
+      <c r="F848" t="inlineStr">
+        <is>
+          <t>C:\Users\admin\Documents\ANGIELSKI\Angielski do słuchania\fate.mp3</t>
         </is>
       </c>
       <c r="G848" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H848" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="849" ht="15" customHeight="1" s="5">

</xml_diff>